<commit_message>
Update tasks and gliders
</commit_message>
<xml_diff>
--- a/data/Database.xlsx
+++ b/data/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge69dox\Schlautmann\00_private\01_Flying\WGC_Tabor\Quellen\tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge69dox\Schlautmann\00_private\01_Flying\WGC_Tabor\Quellen\tracking\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A64AC95-5A85-490C-8A79-14A54F64F265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E96271-D617-42DD-B0D5-89DECEFE2F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{9AF3C144-75A6-4A65-8D42-AC6B359BC94F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AF3C144-75A6-4A65-8D42-AC6B359BC94F}"/>
   </bookViews>
   <sheets>
     <sheet name="WGC2025" sheetId="1" r:id="rId1"/>
@@ -3472,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E7876E-E250-4E28-BFB0-5D6337AED830}">
   <dimension ref="A1:L165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3634,7 +3634,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="32.25" thickBot="1">
+    <row r="5" spans="1:12" ht="16.5" thickBot="1">
       <c r="A5" s="4">
         <v>25</v>
       </c>
@@ -3774,7 +3774,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="32.25" thickBot="1">
+    <row r="9" spans="1:12" ht="16.5" thickBot="1">
       <c r="A9" s="4">
         <v>37</v>
       </c>
@@ -3910,7 +3910,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="32.25" thickBot="1">
+    <row r="13" spans="1:12" ht="16.5" thickBot="1">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -3945,7 +3945,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="32.25" thickBot="1">
+    <row r="14" spans="1:12" ht="16.5" thickBot="1">
       <c r="A14" s="4">
         <v>38</v>
       </c>
@@ -4122,7 +4122,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="32.25" thickBot="1">
+    <row r="19" spans="1:12" ht="16.5" thickBot="1">
       <c r="A19" s="4">
         <v>15</v>
       </c>
@@ -4157,7 +4157,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="32.25" thickBot="1">
+    <row r="20" spans="1:12" ht="16.5" thickBot="1">
       <c r="A20" s="4">
         <v>29</v>
       </c>
@@ -4503,7 +4503,7 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" ht="32.25" thickBot="1">
+    <row r="30" spans="1:12" ht="18.75" thickBot="1">
       <c r="A30" s="4">
         <v>7</v>
       </c>
@@ -4538,7 +4538,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" ht="32.25" thickBot="1">
+    <row r="31" spans="1:12" ht="16.5" thickBot="1">
       <c r="A31" s="4">
         <v>23</v>
       </c>
@@ -4571,7 +4571,7 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" ht="32.25" thickBot="1">
+    <row r="32" spans="1:12" ht="16.5" thickBot="1">
       <c r="A32" s="4">
         <v>24</v>
       </c>
@@ -4744,7 +4744,7 @@
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
     </row>
-    <row r="37" spans="1:12" ht="32.25" thickBot="1">
+    <row r="37" spans="1:12" ht="16.5" thickBot="1">
       <c r="A37" s="4">
         <v>18</v>
       </c>
@@ -4779,7 +4779,7 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="1:12" ht="32.25" thickBot="1">
+    <row r="38" spans="1:12" ht="16.5" thickBot="1">
       <c r="A38" s="4">
         <v>19</v>
       </c>
@@ -4977,15 +4977,17 @@
       <c r="H43" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="I43" s="10"/>
+      <c r="I43" s="10" t="s">
+        <v>538</v>
+      </c>
       <c r="J43" s="10" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[FlarmID]],",,",B43,",",E43," ",C43)</f>
-        <v>,,W,🇩🇰 Michael Mix</v>
+        <v>DDEDF9,,W,🇩🇰 Michael Mix</v>
       </c>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:12" ht="32.25" thickBot="1">
+    <row r="44" spans="1:12" ht="16.5" thickBot="1">
       <c r="A44" s="4">
         <v>9</v>
       </c>
@@ -5020,7 +5022,7 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:12" ht="32.25" thickBot="1">
+    <row r="45" spans="1:12" ht="16.5" thickBot="1">
       <c r="A45" s="4">
         <v>10</v>
       </c>
@@ -5230,7 +5232,7 @@
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
-    <row r="51" spans="1:12" ht="32.25" thickBot="1">
+    <row r="51" spans="1:12" ht="16.5" thickBot="1">
       <c r="A51" s="4">
         <v>17</v>
       </c>
@@ -5265,7 +5267,7 @@
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
     </row>
-    <row r="52" spans="1:12" ht="32.25" thickBot="1">
+    <row r="52" spans="1:12" ht="16.5" thickBot="1">
       <c r="A52" s="4">
         <v>26</v>
       </c>
@@ -5512,7 +5514,7 @@
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" ht="32.25" thickBot="1">
+    <row r="59" spans="1:12" ht="16.5" thickBot="1">
       <c r="A59" s="4">
         <v>8</v>
       </c>
@@ -5605,12 +5607,10 @@
       <c r="H61" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="I61" s="9" t="s">
-        <v>538</v>
-      </c>
+      <c r="I61" s="9"/>
       <c r="J61" s="10" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[FlarmID]],",,",B61,",",E61," ",C61)</f>
-        <v>DDEDF9,,KW,🇫🇷 Maximilian SEIS</v>
+        <v>,,KW,🇫🇷 Maximilian SEIS</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
@@ -5685,7 +5685,7 @@
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
     </row>
-    <row r="64" spans="1:12" ht="32.25" thickBot="1">
+    <row r="64" spans="1:12" ht="16.5" thickBot="1">
       <c r="A64" s="4">
         <v>14</v>
       </c>
@@ -5720,7 +5720,7 @@
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
     </row>
-    <row r="65" spans="1:12" ht="32.25" thickBot="1">
+    <row r="65" spans="1:12" ht="16.5" thickBot="1">
       <c r="A65" s="4">
         <v>16</v>
       </c>
@@ -6000,7 +6000,7 @@
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
     </row>
-    <row r="73" spans="1:12" ht="32.25" thickBot="1">
+    <row r="73" spans="1:12" ht="16.5" thickBot="1">
       <c r="A73" s="4">
         <v>36</v>
       </c>
@@ -6103,7 +6103,7 @@
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
     </row>
-    <row r="76" spans="1:12" ht="32.25" thickBot="1">
+    <row r="76" spans="1:12" ht="16.5" thickBot="1">
       <c r="A76" s="4">
         <v>20</v>
       </c>
@@ -6138,7 +6138,7 @@
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
     </row>
-    <row r="77" spans="1:12" ht="32.25" thickBot="1">
+    <row r="77" spans="1:12" ht="16.5" thickBot="1">
       <c r="A77" s="4">
         <v>22</v>
       </c>
@@ -6243,7 +6243,7 @@
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
     </row>
-    <row r="80" spans="1:12" ht="32.25" thickBot="1">
+    <row r="80" spans="1:12" ht="16.5" thickBot="1">
       <c r="A80" s="4">
         <v>6</v>
       </c>
@@ -6449,7 +6449,7 @@
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
     </row>
-    <row r="86" spans="1:12" ht="32.25" thickBot="1">
+    <row r="86" spans="1:12" ht="16.5" thickBot="1">
       <c r="A86" s="4">
         <v>27</v>
       </c>
@@ -6484,7 +6484,7 @@
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
     </row>
-    <row r="87" spans="1:12" ht="32.25" thickBot="1">
+    <row r="87" spans="1:12" ht="16.5" thickBot="1">
       <c r="A87" s="4">
         <v>34</v>
       </c>
@@ -6657,7 +6657,7 @@
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
     </row>
-    <row r="92" spans="1:12" ht="32.25" thickBot="1">
+    <row r="92" spans="1:12" ht="16.5" thickBot="1">
       <c r="A92" s="4">
         <v>30</v>
       </c>
@@ -6692,7 +6692,7 @@
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
     </row>
-    <row r="93" spans="1:12" ht="32.25" thickBot="1">
+    <row r="93" spans="1:12" ht="16.5" thickBot="1">
       <c r="A93" s="4">
         <v>35</v>
       </c>
@@ -6902,7 +6902,7 @@
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
     </row>
-    <row r="99" spans="1:12" ht="32.25" thickBot="1">
+    <row r="99" spans="1:12" ht="16.5" thickBot="1">
       <c r="A99" s="4">
         <v>2</v>
       </c>
@@ -6935,7 +6935,7 @@
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
     </row>
-    <row r="100" spans="1:12" ht="32.25" thickBot="1">
+    <row r="100" spans="1:12" ht="16.5" thickBot="1">
       <c r="A100" s="4">
         <v>3</v>
       </c>
@@ -7110,7 +7110,7 @@
       </c>
       <c r="L104" s="4"/>
     </row>
-    <row r="105" spans="1:12" ht="32.25" thickBot="1">
+    <row r="105" spans="1:12" ht="16.5" thickBot="1">
       <c r="A105" s="4">
         <v>28</v>
       </c>
@@ -7143,7 +7143,7 @@
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
     </row>
-    <row r="106" spans="1:12" ht="32.25" thickBot="1">
+    <row r="106" spans="1:12" ht="16.5" thickBot="1">
       <c r="A106" s="4">
         <v>32</v>
       </c>
@@ -7310,7 +7310,7 @@
       <c r="K110" s="4"/>
       <c r="L110" s="4"/>
     </row>
-    <row r="111" spans="1:12" ht="32.25" thickBot="1">
+    <row r="111" spans="1:12" ht="16.5" thickBot="1">
       <c r="A111" s="4">
         <v>4</v>
       </c>

</xml_diff>